<commit_message>
Updated bugs and queries xls following more testing, Added help text for miscellaneous page.
</commit_message>
<xml_diff>
--- a/editor/ldmledit bugs and queries.xlsx
+++ b/editor/ldmledit bugs and queries.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Page</t>
   </si>
@@ -167,12 +167,24 @@
   <si>
     <t>NB: I've added help text to the loadnsave page</t>
   </si>
+  <si>
+    <t>New help text still isn't showing up</t>
+  </si>
+  <si>
+    <t>Line Direction and Yes/No info is now being saved, but it isn't displayed when the locale is loaded</t>
+  </si>
+  <si>
+    <t>Most of the above looks to be working now - thanks!</t>
+  </si>
+  <si>
+    <t>I've now also added help text to the misc page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -210,6 +222,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -231,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -252,12 +283,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -648,193 +683,231 @@
       <c r="B5" s="6">
         <v>42010</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="6">
+        <v>42013</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B7" s="6">
         <v>41995</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6">
+    <row r="8" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6">
         <v>42010</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B9" s="6">
         <v>41995</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="6">
+    <row r="10" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="6">
         <v>42010</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="6">
-        <v>41995</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B11" s="6">
-        <v>41995</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>42013</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="6">
+        <v>41995</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6">
+        <v>41995</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="6">
         <v>42006</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3"/>
-    </row>
-    <row r="15" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="B15" s="6">
-        <v>41995</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="69" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="6">
-        <v>42006</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="B17" s="6">
         <v>41995</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="69" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="6">
+        <v>42006</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="6">
+        <v>41995</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="9">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
         <v>42010</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C21" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
+        <v>42013</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>42013</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Update Bugs & Queries list, Change language and script prompts.
</commit_message>
<xml_diff>
--- a/editor/ldmledit bugs and queries.xlsx
+++ b/editor/ldmledit bugs and queries.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="21Jan15_archive" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>Page</t>
   </si>
@@ -179,12 +180,43 @@
   <si>
     <t>I've now also added help text to the misc page</t>
   </si>
+  <si>
+    <t>This works perfectly for loading from, and saving to, a local file; it doesn't work when fetching a file from the SLDR.  Ideally it should also be updated when someone changes the language id or script id and clicks on the &lt;Save&gt; button. That way it will always show the id of the locale you're going to save.</t>
+  </si>
+  <si>
+    <t>There is a similar issue with languages which have both a 2-character ISO code (eg te) and a 3-character code (eg tel).  Potentially we could end up with two different files for the same locale.
+I'm wondering whether we should 'normalise' the locale id (eg by referencing likely subtags), so if someone keys in language: tel and script: Latn, it will be normalised from tel_Latn to te.</t>
+  </si>
+  <si>
+    <t>ANRCC request: It would be nice if the language and script codes could be selected from drop-down boxes, instead of being free text.</t>
+  </si>
+  <si>
+    <t>Page links tidied up and pushed: s.s.o. needs updating</t>
+  </si>
+  <si>
+    <t>Prompts changed: changes need committing</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>ANRCC request: it would be better if links to ldml spec pages opened in a new window. (I chgd thehtml, but it didn't seem to help.)</t>
+  </si>
+  <si>
+    <t>dates</t>
+  </si>
+  <si>
+    <t>ANRCC request: Make simpler dates page, with just a few prompts</t>
+  </si>
+  <si>
+    <t>It would be valuable if a parent locale could be specified on the loadnsave page (eg Telugu for Gondi)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -241,6 +273,30 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -292,6 +348,33 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -595,29 +678,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="14.44140625"/>
-    <col min="3" max="3" width="85.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625"/>
+    <col min="2" max="2" width="14.44140625" style="18"/>
+    <col min="3" max="3" width="85.109375" style="19" customWidth="1"/>
     <col min="4" max="4" width="53.5546875" customWidth="1"/>
     <col min="5" max="9" width="93.109375"/>
     <col min="10" max="1025" width="14.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1"/>
@@ -644,6 +728,246 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16">
+        <v>42006</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="16">
+        <v>41995</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="41.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="16">
+        <v>42026</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" ht="69" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="16">
+        <v>42006</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="16">
+        <v>41995</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="17">
+        <v>42026</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="17">
+        <v>42025</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="17">
+        <v>42025</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="17">
+        <v>42026</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="17">
+        <v>42026</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="17">
+        <v>42026</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="17">
+        <v>42026</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.77734375" customWidth="1"/>
+    <col min="3" max="3" width="85.109375" customWidth="1"/>
+    <col min="4" max="4" width="53.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+    </row>
     <row r="2" spans="1:26" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>

</xml_diff>